<commit_message>
Common: Added experimental support for atomizer tags
</commit_message>
<xml_diff>
--- a/upgrade/fixtures/tags.xlsx
+++ b/upgrade/fixtures/tags.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\upgrade\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28AF576C-72D6-4324-8CA1-2B572130E61A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{118FF9A7-34FB-4D58-B7D1-DD9D378FEC7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2010" yWindow="7965" windowWidth="23955" windowHeight="13320" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tabs" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="22">
   <si>
     <t>Edde\Tag\Import\TagImport</t>
   </si>
@@ -77,6 +77,21 @@
   </si>
   <si>
     <t>sort</t>
+  </si>
+  <si>
+    <t>mtl</t>
+  </si>
+  <si>
+    <t>draw</t>
+  </si>
+  <si>
+    <t>rmtl</t>
+  </si>
+  <si>
+    <t>dl</t>
+  </si>
+  <si>
+    <t>rdl</t>
   </si>
 </sst>
 </file>
@@ -450,10 +465,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{155FFD59-B00A-42A0-9723-B6B17686BDEE}">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -573,6 +588,50 @@
         <v>8</v>
       </c>
     </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Common: Added filter for plots
</commit_message>
<xml_diff>
--- a/upgrade/fixtures/tags.xlsx
+++ b/upgrade/fixtures/tags.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\upgrade\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{118FF9A7-34FB-4D58-B7D1-DD9D378FEC7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02C09F73-5E28-4BE9-A452-60E175396A15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8250" yWindow="3150" windowWidth="33615" windowHeight="18390" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tabs" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="23">
   <si>
     <t>Edde\Tag\Import\TagImport</t>
   </si>
@@ -92,6 +92,9 @@
   </si>
   <si>
     <t>rdl</t>
+  </si>
+  <si>
+    <t>omtl</t>
   </si>
 </sst>
 </file>
@@ -465,10 +468,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{155FFD59-B00A-42A0-9723-B6B17686BDEE}">
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -590,7 +593,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B11" t="s">
         <v>18</v>
@@ -601,7 +604,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B12" t="s">
         <v>18</v>
@@ -612,7 +615,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B13" t="s">
         <v>18</v>
@@ -630,6 +633,17 @@
       </c>
       <c r="C14">
         <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>20</v>
+      </c>
+      <c r="B15" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: Added cells to mods
</commit_message>
<xml_diff>
--- a/upgrade/fixtures/tags.xlsx
+++ b/upgrade/fixtures/tags.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\upgrade\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02C09F73-5E28-4BE9-A452-60E175396A15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{739E5BBD-4E70-498D-AAF4-BB2AEB6DB408}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8250" yWindow="3150" windowWidth="33615" windowHeight="18390" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6015" yWindow="2280" windowWidth="33615" windowHeight="18390" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tabs" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="24">
   <si>
     <t>Edde\Tag\Import\TagImport</t>
   </si>
@@ -95,6 +95,9 @@
   </si>
   <si>
     <t>omtl</t>
+  </si>
+  <si>
+    <t>cell-type</t>
   </si>
 </sst>
 </file>
@@ -468,10 +471,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{155FFD59-B00A-42A0-9723-B6B17686BDEE}">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -646,6 +649,61 @@
         <v>4</v>
       </c>
     </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>18350</v>
+      </c>
+      <c r="B16" t="s">
+        <v>23</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>18650</v>
+      </c>
+      <c r="B17" t="s">
+        <v>23</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>20700</v>
+      </c>
+      <c r="B18" t="s">
+        <v>23</v>
+      </c>
+      <c r="C18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>21700</v>
+      </c>
+      <c r="B19" t="s">
+        <v>23</v>
+      </c>
+      <c r="C19">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>26650</v>
+      </c>
+      <c r="B20" t="s">
+        <v>23</v>
+      </c>
+      <c r="C20">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Common: Added atomizer type
</commit_message>
<xml_diff>
--- a/upgrade/fixtures/tags.xlsx
+++ b/upgrade/fixtures/tags.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\upgrade\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{739E5BBD-4E70-498D-AAF4-BB2AEB6DB408}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A55FB46-D45B-4C7B-90F6-55928FAD31FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6015" yWindow="2280" windowWidth="33615" windowHeight="18390" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="28">
   <si>
     <t>Edde\Tag\Import\TagImport</t>
   </si>
@@ -98,6 +98,18 @@
   </si>
   <si>
     <t>cell-type</t>
+  </si>
+  <si>
+    <t>atomizer-type</t>
+  </si>
+  <si>
+    <t>RTA</t>
+  </si>
+  <si>
+    <t>RDA</t>
+  </si>
+  <si>
+    <t>RDTA</t>
   </si>
 </sst>
 </file>
@@ -471,10 +483,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{155FFD59-B00A-42A0-9723-B6B17686BDEE}">
-  <dimension ref="A1:C20"/>
+  <dimension ref="A1:C23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -704,6 +716,39 @@
         <v>4</v>
       </c>
     </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>25</v>
+      </c>
+      <c r="B21" t="s">
+        <v>24</v>
+      </c>
+      <c r="C21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>26</v>
+      </c>
+      <c r="B22" t="s">
+        <v>24</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>27</v>
+      </c>
+      <c r="B23" t="s">
+        <v>24</v>
+      </c>
+      <c r="C23">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>